<commit_message>
Update Plan de Control y Seguimiento -5122019.xlsx
</commit_message>
<xml_diff>
--- a/Documentación (Avances)/Primera Iteración/Plan de Control y Seguimiento -5122019.xlsx
+++ b/Documentación (Avances)/Primera Iteración/Plan de Control y Seguimiento -5122019.xlsx
@@ -1,18 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\torre\OneDrive\Documentos\GitHub\portafolio\Documentación (Avances)\Primera Iteración\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_274F3871D0565FB5533E8EFDCF038DC3CA0A8762" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2EFD2BBC-B4C4-4262-9BE5-93967F3A3E30}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 Iteración" sheetId="1" r:id="rId1"/>
     <sheet name="2 Iteración" sheetId="2" r:id="rId2"/>
     <sheet name="3 Iteración" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -21,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="86">
   <si>
     <t>Nombre del proyecto</t>
   </si>
@@ -77,9 +91,6 @@
     <t>Diagrama EDT</t>
   </si>
   <si>
-    <t>Diccionario EDT</t>
-  </si>
-  <si>
     <t>Carta Gantt</t>
   </si>
   <si>
@@ -203,9 +214,6 @@
     <t>Informe de Cierre</t>
   </si>
   <si>
-    <t>Manual de Usuario por Perfiles</t>
-  </si>
-  <si>
     <t>Manual Tecnico del Sistema de Escritorio</t>
   </si>
   <si>
@@ -236,12 +244,6 @@
     <t xml:space="preserve">Grupo </t>
   </si>
   <si>
-    <t>Roberto Gonzalez, Renzo Espeleta , Manuel Torres</t>
-  </si>
-  <si>
-    <t>Roberto Gonzalez,Renzo Espeleta</t>
-  </si>
-  <si>
     <t>Grupo</t>
   </si>
   <si>
@@ -285,12 +287,18 @@
   </si>
   <si>
     <t>Informe de Resultado de Pruebas escritorio</t>
+  </si>
+  <si>
+    <t>Manual de Usuario por Perfiles web</t>
+  </si>
+  <si>
+    <t>Manual de Usuario por Perfiles Escritorio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
@@ -765,20 +773,20 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1120,60 +1128,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="38.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.25" style="16" customWidth="1"/>
-    <col min="3" max="4" width="15.75" style="22" customWidth="1"/>
-    <col min="5" max="5" width="15.125" style="35" customWidth="1"/>
-    <col min="6" max="6" width="15.625" style="32" customWidth="1"/>
-    <col min="7" max="7" width="25.625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="38.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.19921875" style="16" customWidth="1"/>
+    <col min="3" max="4" width="15.69921875" style="22" customWidth="1"/>
+    <col min="5" max="5" width="15.09765625" style="35" customWidth="1"/>
+    <col min="6" max="6" width="15.59765625" style="32" customWidth="1"/>
+    <col min="7" max="7" width="25.59765625" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" thickBot="1"/>
+    <row r="1" spans="1:7" ht="16.2" thickBot="1"/>
     <row r="2" spans="1:7" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="67" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="68" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="70">
-        <f>COUNTIF(G8:G34,"OK")</f>
-        <v>15</v>
-      </c>
-      <c r="F2" s="69" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="70">
-        <f>COUNTIF(G8:G34,"Pendiente")</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="16.5" thickTop="1"/>
+      <c r="B2" s="71" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="71"/>
+      <c r="D2" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="69">
+        <f>COUNTIF(G8:G33,"OK")</f>
+        <v>17</v>
+      </c>
+      <c r="F2" s="68" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="69">
+        <f>COUNTIF(G8:G33,"Pendiente")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16.2" thickTop="1"/>
     <row r="4" spans="1:7" ht="15.75" hidden="1" customHeight="1">
-      <c r="D4" s="69" t="s">
+      <c r="D4" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="71">
+      <c r="E4" s="70">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="22.15" customHeight="1">
+    <row r="5" spans="1:7" ht="22.2" customHeight="1">
       <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
@@ -1209,7 +1217,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="24"/>
@@ -1220,10 +1228,10 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>8</v>
@@ -1238,15 +1246,15 @@
         <v>43735</v>
       </c>
       <c r="G8" s="55" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>8</v>
@@ -1261,7 +1269,7 @@
         <v>43735</v>
       </c>
       <c r="G9" s="55" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1269,7 +1277,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C10" s="50" t="s">
         <v>8</v>
@@ -1284,15 +1292,15 @@
         <v>43755</v>
       </c>
       <c r="G10" s="55" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="48" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C11" s="50" t="s">
         <v>8</v>
@@ -1307,7 +1315,7 @@
         <v>43754</v>
       </c>
       <c r="G11" s="55" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1315,7 +1323,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="49" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C12" s="50" t="s">
         <v>8</v>
@@ -1330,7 +1338,7 @@
         <v>43762</v>
       </c>
       <c r="G12" s="55" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1338,68 +1346,68 @@
         <v>18</v>
       </c>
       <c r="B13" s="49" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C13" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="54" t="s">
-        <v>69</v>
+      <c r="D13" s="50" t="s">
+        <v>11</v>
       </c>
       <c r="E13" s="51">
-        <v>43759</v>
+        <v>43752</v>
       </c>
       <c r="F13" s="52">
-        <v>43763</v>
-      </c>
-      <c r="G13" s="66" t="s">
-        <v>76</v>
+        <v>43755</v>
+      </c>
+      <c r="G13" s="55" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="50" t="s">
+      <c r="A14" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="51">
-        <v>43752</v>
-      </c>
-      <c r="F14" s="52">
-        <v>43755</v>
-      </c>
-      <c r="G14" s="66" t="s">
-        <v>76</v>
+      <c r="E14" s="38">
+        <v>43703</v>
+      </c>
+      <c r="F14" s="42">
+        <v>43735</v>
+      </c>
+      <c r="G14" s="55" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C15" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="50" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="38">
-        <v>43703</v>
+        <v>43752</v>
       </c>
       <c r="F15" s="42">
-        <v>43735</v>
+        <v>43756</v>
       </c>
       <c r="G15" s="55" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1407,22 +1415,22 @@
         <v>25</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C16" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="50" t="s">
+      <c r="D16" s="25" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="38">
-        <v>43752</v>
+        <v>43735</v>
       </c>
       <c r="F16" s="42">
-        <v>43756</v>
+        <v>43738</v>
       </c>
       <c r="G16" s="55" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1430,22 +1438,18 @@
         <v>26</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="C17" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="38">
-        <v>43735</v>
-      </c>
-      <c r="F17" s="42">
-        <v>43738</v>
-      </c>
-      <c r="G17" s="55" t="s">
-        <v>75</v>
+      <c r="D17" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="38"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="66" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1453,71 +1457,75 @@
         <v>27</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="54" t="s">
-        <v>69</v>
+      <c r="D18" s="25" t="s">
+        <v>11</v>
       </c>
       <c r="E18" s="38"/>
       <c r="F18" s="42"/>
-      <c r="G18" s="66" t="s">
-        <v>76</v>
+      <c r="G18" s="55" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="25" t="s">
+      <c r="B19" s="18"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="18"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="38"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="55" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="10" t="s">
+      <c r="E20" s="38">
+        <v>43731</v>
+      </c>
+      <c r="F20" s="42">
+        <v>43735</v>
+      </c>
+      <c r="G20" s="55" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="18"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="38">
-        <v>43731</v>
-      </c>
-      <c r="F21" s="42">
-        <v>43735</v>
-      </c>
-      <c r="G21" s="55" t="s">
-        <v>75</v>
+      <c r="B21" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="51">
+        <v>43752</v>
+      </c>
+      <c r="F21" s="52">
+        <v>43756</v>
+      </c>
+      <c r="G21" s="66" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1525,22 +1533,22 @@
         <v>30</v>
       </c>
       <c r="B22" s="49" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C22" s="50" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="54" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E22" s="51">
         <v>43752</v>
       </c>
       <c r="F22" s="52">
-        <v>43756</v>
+        <v>43755</v>
       </c>
       <c r="G22" s="66" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1548,22 +1556,22 @@
         <v>31</v>
       </c>
       <c r="B23" s="49" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C23" s="50" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="54" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E23" s="51">
         <v>43752</v>
       </c>
       <c r="F23" s="52">
-        <v>43755</v>
+        <v>43758</v>
       </c>
       <c r="G23" s="66" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1571,13 +1579,13 @@
         <v>32</v>
       </c>
       <c r="B24" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="54" t="s">
         <v>67</v>
-      </c>
-      <c r="C24" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="54" t="s">
-        <v>69</v>
       </c>
       <c r="E24" s="51">
         <v>43752</v>
@@ -1586,7 +1594,7 @@
         <v>43758</v>
       </c>
       <c r="G24" s="66" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1594,96 +1602,96 @@
         <v>33</v>
       </c>
       <c r="B25" s="49" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C25" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="54" t="s">
-        <v>69</v>
+      <c r="D25" s="25" t="s">
+        <v>11</v>
       </c>
       <c r="E25" s="51">
         <v>43752</v>
       </c>
       <c r="F25" s="52">
-        <v>43758</v>
-      </c>
-      <c r="G25" s="66" t="s">
-        <v>76</v>
+        <v>43755</v>
+      </c>
+      <c r="G25" s="55" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="53" t="s">
+      <c r="A26" s="11"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="19"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="54" t="s">
-        <v>69</v>
-      </c>
-      <c r="E26" s="51">
-        <v>43752</v>
-      </c>
-      <c r="F26" s="52">
-        <v>43755</v>
-      </c>
-      <c r="G26" s="66" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="11"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="19"/>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="10" t="s">
+      <c r="B27" s="20"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="20"/>
+    </row>
+    <row r="28" spans="1:7" ht="31.2">
+      <c r="A28" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="20"/>
-    </row>
-    <row r="29" spans="1:7" ht="31.5">
-      <c r="A29" s="14" t="s">
+      <c r="B28" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="C28" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="38">
+        <v>43703</v>
+      </c>
+      <c r="F28" s="42">
+        <v>43721</v>
+      </c>
+      <c r="G28" s="55" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="31.2">
+      <c r="A29" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="B29" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="50" t="s">
         <v>8</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E29" s="38">
-        <v>43703</v>
-      </c>
-      <c r="F29" s="42">
-        <v>43721</v>
+      <c r="E29" s="51">
+        <v>43722</v>
+      </c>
+      <c r="F29" s="52">
+        <v>43768</v>
       </c>
       <c r="G29" s="55" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="31.5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="31.2">
       <c r="A30" s="56" t="s">
         <v>38</v>
       </c>
       <c r="B30" s="49" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30" s="50" t="s">
         <v>8</v>
@@ -1698,15 +1706,15 @@
         <v>43768</v>
       </c>
       <c r="G30" s="55" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="31.5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="31.2">
       <c r="A31" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="49" t="s">
-        <v>37</v>
+      <c r="B31" s="19" t="s">
+        <v>62</v>
       </c>
       <c r="C31" s="50" t="s">
         <v>8</v>
@@ -1715,93 +1723,70 @@
         <v>11</v>
       </c>
       <c r="E31" s="51">
-        <v>43722</v>
+        <v>43752</v>
       </c>
       <c r="F31" s="52">
-        <v>43768</v>
+        <v>43756</v>
       </c>
       <c r="G31" s="55" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="31.5">
-      <c r="A32" s="56" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="31.2">
+      <c r="A32" s="14" t="s">
         <v>40</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="51">
-        <v>43752</v>
-      </c>
-      <c r="F32" s="52">
-        <v>43756</v>
-      </c>
-      <c r="G32" s="55" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="31.5">
+        <v>62</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="38"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="66" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="31.2">
       <c r="A33" s="14" t="s">
         <v>41</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C33" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="54" t="s">
-        <v>9</v>
+      <c r="D33" s="25" t="s">
+        <v>11</v>
       </c>
       <c r="E33" s="38"/>
       <c r="F33" s="42"/>
-      <c r="G33" s="66" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="31.5">
-      <c r="A34" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" s="25" t="s">
-        <v>11</v>
-      </c>
+      <c r="G33" s="55" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="14"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
       <c r="E34" s="38"/>
       <c r="F34" s="42"/>
-      <c r="G34" s="55" t="s">
-        <v>75</v>
-      </c>
+      <c r="G34" s="19"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="14"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="19"/>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="15"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="28"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="31"/>
+      <c r="A35" s="15"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1818,53 +1803,53 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="43.875" style="22" customWidth="1"/>
-    <col min="2" max="2" width="16.25" style="16" customWidth="1"/>
-    <col min="3" max="4" width="15.75" style="22" customWidth="1"/>
-    <col min="5" max="5" width="15.125" style="35" customWidth="1"/>
-    <col min="6" max="6" width="12.75" style="32" customWidth="1"/>
-    <col min="7" max="7" width="17.25" style="16" customWidth="1"/>
+    <col min="1" max="1" width="43.8984375" style="22" customWidth="1"/>
+    <col min="2" max="2" width="16.19921875" style="16" customWidth="1"/>
+    <col min="3" max="4" width="15.69921875" style="22" customWidth="1"/>
+    <col min="5" max="5" width="15.09765625" style="35" customWidth="1"/>
+    <col min="6" max="6" width="12.69921875" style="32" customWidth="1"/>
+    <col min="7" max="7" width="17.19921875" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" thickBot="1"/>
-    <row r="2" spans="1:7" ht="20.25" thickTop="1" thickBot="1">
+    <row r="1" spans="1:7" ht="16.2" thickBot="1"/>
+    <row r="2" spans="1:7" ht="19.2" thickTop="1" thickBot="1">
       <c r="A2" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="68" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="70">
-        <f>COUNTIF(D8:D38,"OK")</f>
-        <v>7</v>
-      </c>
-      <c r="F2" s="69" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="70">
-        <f>COUNTIF(D8:D38,"Pendiente")</f>
+      <c r="C2" s="71"/>
+      <c r="D2" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="69">
+        <f>COUNTIF(D8:D39,"OK")</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="16.5" thickTop="1"/>
+      <c r="F2" s="68" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="69">
+        <f>COUNTIF(D8:D39,"Pendiente")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16.2" thickTop="1"/>
     <row r="4" spans="1:7" hidden="1"/>
-    <row r="5" spans="1:7" ht="22.15" customHeight="1">
+    <row r="5" spans="1:7" ht="22.2" customHeight="1">
       <c r="A5" s="59" t="s">
         <v>1</v>
       </c>
@@ -1900,7 +1885,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="61" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="24"/>
@@ -1911,16 +1896,16 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="62" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E8" s="38"/>
       <c r="F8" s="42"/>
@@ -1928,16 +1913,16 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="62" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E9" s="38"/>
       <c r="F9" s="42"/>
@@ -1945,16 +1930,16 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E10" s="38"/>
       <c r="F10" s="42"/>
@@ -1962,16 +1947,16 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E11" s="38"/>
       <c r="F11" s="42"/>
@@ -1979,16 +1964,16 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E12" s="38"/>
       <c r="F12" s="42"/>
@@ -1996,16 +1981,16 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="57" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E13" s="38"/>
       <c r="F13" s="42"/>
@@ -2013,16 +1998,16 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="57" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C14" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E14" s="38"/>
       <c r="F14" s="42"/>
@@ -2030,14 +2015,14 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="63" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E15" s="38"/>
       <c r="F15" s="42"/>
@@ -2045,7 +2030,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="61" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="24"/>
@@ -2054,35 +2039,35 @@
       <c r="F16" s="41"/>
       <c r="G16" s="18"/>
     </row>
-    <row r="17" spans="1:7" ht="47.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="57" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="C17" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="29" t="s">
-        <v>76</v>
+      <c r="D17" s="25" t="s">
+        <v>71</v>
       </c>
       <c r="E17" s="38"/>
       <c r="F17" s="42"/>
       <c r="G17" s="19"/>
     </row>
-    <row r="18" spans="1:7" ht="47.25">
-      <c r="A18" s="63" t="s">
-        <v>61</v>
+    <row r="18" spans="1:7">
+      <c r="A18" s="57" t="s">
+        <v>85</v>
       </c>
       <c r="B18" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="29" t="s">
         <v>72</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>76</v>
       </c>
       <c r="E18" s="38"/>
       <c r="F18" s="42"/>
@@ -2090,70 +2075,70 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="19" t="s">
-        <v>37</v>
-      </c>
       <c r="C19" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E19" s="38"/>
       <c r="F19" s="42"/>
       <c r="G19" s="19"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="62"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
+      <c r="A20" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>71</v>
+      </c>
       <c r="E20" s="38"/>
       <c r="F20" s="42"/>
       <c r="G20" s="19"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="61" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="20"/>
+      <c r="A21" s="62"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="19"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="64" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="E22" s="38"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="44"/>
+      <c r="A22" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="20"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="20"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="64" t="s">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="C23" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="25" t="s">
-        <v>75</v>
+      <c r="D23" s="29" t="s">
+        <v>72</v>
       </c>
       <c r="E23" s="38"/>
       <c r="F23" s="42"/>
@@ -2161,33 +2146,33 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="64" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="C24" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="29" t="s">
-        <v>76</v>
+      <c r="D24" s="25" t="s">
+        <v>71</v>
       </c>
       <c r="E24" s="38"/>
       <c r="F24" s="42"/>
-      <c r="G24" s="19"/>
+      <c r="G24" s="44"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="64" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="C25" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E25" s="38"/>
       <c r="F25" s="42"/>
@@ -2195,16 +2180,16 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="64" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="C26" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="29" t="s">
-        <v>76</v>
+      <c r="D26" s="25" t="s">
+        <v>71</v>
       </c>
       <c r="E26" s="38"/>
       <c r="F26" s="42"/>
@@ -2212,16 +2197,16 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="64" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="C27" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E27" s="38"/>
       <c r="F27" s="42"/>
@@ -2229,16 +2214,16 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="64" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="C28" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="29" t="s">
-        <v>76</v>
+      <c r="D28" s="25" t="s">
+        <v>71</v>
       </c>
       <c r="E28" s="38"/>
       <c r="F28" s="42"/>
@@ -2246,29 +2231,46 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="64" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C29" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="29" t="s">
-        <v>76</v>
+      <c r="D29" s="25" t="s">
+        <v>71</v>
       </c>
       <c r="E29" s="38"/>
       <c r="F29" s="42"/>
       <c r="G29" s="19"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="65"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="31"/>
+      <c r="A30" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" s="38"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="19"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="65"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2280,57 +2282,57 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="40.625" style="45" customWidth="1"/>
-    <col min="2" max="2" width="16.25" style="16" customWidth="1"/>
-    <col min="3" max="4" width="15.75" style="22" customWidth="1"/>
-    <col min="5" max="5" width="15.125" style="35" customWidth="1"/>
-    <col min="6" max="6" width="12.75" style="32" customWidth="1"/>
+    <col min="1" max="1" width="40.59765625" style="45" customWidth="1"/>
+    <col min="2" max="2" width="16.19921875" style="16" customWidth="1"/>
+    <col min="3" max="4" width="15.69921875" style="22" customWidth="1"/>
+    <col min="5" max="5" width="15.09765625" style="35" customWidth="1"/>
+    <col min="6" max="6" width="12.69921875" style="32" customWidth="1"/>
     <col min="7" max="7" width="14" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" thickBot="1">
+    <row r="1" spans="1:7" ht="16.2" thickBot="1">
       <c r="A1" s="22"/>
     </row>
-    <row r="2" spans="1:7" ht="20.25" thickTop="1" thickBot="1">
+    <row r="2" spans="1:7" ht="19.2" thickTop="1" thickBot="1">
       <c r="A2" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="68" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="70">
+      <c r="C2" s="71"/>
+      <c r="D2" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="69">
         <f>COUNTIF(D8:D38,"OK")</f>
-        <v>6</v>
-      </c>
-      <c r="F2" s="69" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="70">
+        <v>9</v>
+      </c>
+      <c r="F2" s="68" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="69">
         <f>COUNTIF(D8:D38,"Pendiente")</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="16.5" thickTop="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16.2" thickTop="1">
       <c r="A3" s="22"/>
     </row>
     <row r="4" spans="1:7" hidden="1"/>
-    <row r="5" spans="1:7" ht="22.15" customHeight="1">
+    <row r="5" spans="1:7" ht="22.2" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -2366,7 +2368,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="24"/>
@@ -2377,16 +2379,16 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E8" s="38"/>
       <c r="F8" s="42"/>
@@ -2394,16 +2396,16 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E9" s="38"/>
       <c r="F9" s="42"/>
@@ -2411,16 +2413,16 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E10" s="38"/>
       <c r="F10" s="42"/>
@@ -2428,14 +2430,14 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E11" s="38"/>
       <c r="F11" s="42"/>
@@ -2443,14 +2445,14 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="19"/>
       <c r="C12" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E12" s="38"/>
       <c r="F12" s="42"/>
@@ -2458,16 +2460,16 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E13" s="38"/>
       <c r="F13" s="42"/>
@@ -2484,7 +2486,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="24"/>
@@ -2495,14 +2497,14 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E16" s="38"/>
       <c r="F16" s="42"/>
@@ -2510,14 +2512,14 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E17" s="38"/>
       <c r="F17" s="42"/>
@@ -2525,16 +2527,16 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C18" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E18" s="38"/>
       <c r="F18" s="42"/>
@@ -2542,16 +2544,16 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C19" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E19" s="38"/>
       <c r="F19" s="42"/>
@@ -2568,7 +2570,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" s="20"/>
       <c r="C21" s="27"/>
@@ -2579,14 +2581,14 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" s="19"/>
       <c r="C22" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E22" s="38"/>
       <c r="F22" s="42"/>
@@ -2594,14 +2596,14 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" s="19"/>
       <c r="C23" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="55" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E23" s="38"/>
       <c r="F23" s="42"/>
@@ -2609,14 +2611,14 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24" s="19"/>
       <c r="C24" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D24" s="55" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E24" s="38"/>
       <c r="F24" s="42"/>
@@ -2624,14 +2626,14 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B25" s="19"/>
       <c r="C25" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D25" s="55" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E25" s="38"/>
       <c r="F25" s="42"/>
@@ -2639,14 +2641,14 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B26" s="19"/>
       <c r="C26" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="29" t="s">
-        <v>76</v>
+      <c r="D26" s="55" t="s">
+        <v>71</v>
       </c>
       <c r="E26" s="38"/>
       <c r="F26" s="42"/>
@@ -2654,14 +2656,14 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B27" s="19"/>
       <c r="C27" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="55" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E27" s="38"/>
       <c r="F27" s="42"/>
@@ -2669,14 +2671,14 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B28" s="19"/>
       <c r="C28" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="29" t="s">
-        <v>76</v>
+      <c r="D28" s="55" t="s">
+        <v>71</v>
       </c>
       <c r="E28" s="38"/>
       <c r="F28" s="42"/>
@@ -2684,14 +2686,14 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B29" s="19"/>
       <c r="C29" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D29" s="55" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E29" s="38"/>
       <c r="F29" s="42"/>
@@ -2699,14 +2701,14 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="29" t="s">
-        <v>76</v>
+      <c r="D30" s="55" t="s">
+        <v>71</v>
       </c>
       <c r="E30" s="38"/>
       <c r="F30" s="42"/>

</xml_diff>